<commit_message>
Pentester lab Resources added in HackingResources.xlsx
</commit_message>
<xml_diff>
--- a/Hacking Resources.xlsx
+++ b/Hacking Resources.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D326DC45-9F04-4C5F-882B-74D77139C5AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A33330-4E9E-4D3F-A631-C7CC28E8C0A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
   </bookViews>
   <sheets>
     <sheet name="Github" sheetId="1" r:id="rId1"/>
     <sheet name="Hacker One" sheetId="3" r:id="rId2"/>
     <sheet name="Android" sheetId="4" r:id="rId3"/>
     <sheet name="Udacity" sheetId="5" r:id="rId4"/>
-    <sheet name="Udemy" sheetId="2" r:id="rId5"/>
+    <sheet name="Pentester Lab" sheetId="6" r:id="rId5"/>
+    <sheet name="Udemy" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>5 Useful GitHub Repositories #Shorts</t>
   </si>
@@ -140,6 +141,27 @@
   </si>
   <si>
     <t>Intro to BackEnd</t>
+  </si>
+  <si>
+    <t>Android Badge</t>
+  </si>
+  <si>
+    <t>HTTP Badge</t>
+  </si>
+  <si>
+    <t>https://pentesterlab.com/badges/http</t>
+  </si>
+  <si>
+    <t>API Badge</t>
+  </si>
+  <si>
+    <t>https://pentesterlab.com/badges/api</t>
+  </si>
+  <si>
+    <t>Essential Badge</t>
+  </si>
+  <si>
+    <t>https://pentesterlab.com/badges/essential</t>
   </si>
 </sst>
 </file>
@@ -197,13 +219,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -655,7 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C93B1D4-544A-4029-B432-105DE78F91FA}">
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -743,6 +768,58 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114BAD3-2286-4A06-9E26-58D1E6259D0C}">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="53.33203125" customWidth="1"/>
+    <col min="3" max="3" width="70.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7831D5FA-64AA-4534-9A47-34375D983CF8}">
   <dimension ref="B2:B10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Youtube section added. Check some cool OWASP TOP 10 2017 links.
</commit_message>
<xml_diff>
--- a/Hacking Resources.xlsx
+++ b/Hacking Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A33330-4E9E-4D3F-A631-C7CC28E8C0A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FD2F7B-88AC-4F6C-901D-E8946B96BCC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
   </bookViews>
   <sheets>
     <sheet name="Github" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Android" sheetId="4" r:id="rId3"/>
     <sheet name="Udacity" sheetId="5" r:id="rId4"/>
     <sheet name="Pentester Lab" sheetId="6" r:id="rId5"/>
-    <sheet name="Udemy" sheetId="2" r:id="rId6"/>
+    <sheet name="Youtube" sheetId="7" r:id="rId6"/>
+    <sheet name="Udemy" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>5 Useful GitHub Repositories #Shorts</t>
   </si>
@@ -162,6 +163,12 @@
   </si>
   <si>
     <t>https://pentesterlab.com/badges/essential</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLpNYlUeSK_rnsMu5S4UGtGy2HSmZdTUNl</t>
+  </si>
+  <si>
+    <t>OWASP Top 10 2017</t>
   </si>
 </sst>
 </file>
@@ -771,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114BAD3-2286-4A06-9E26-58D1E6259D0C}">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -820,6 +827,33 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771B96C1-7ABF-46C5-9549-9CBFA9D2AE30}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="44.5546875" customWidth="1"/>
+    <col min="3" max="3" width="106.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7831D5FA-64AA-4534-9A47-34375D983CF8}">
   <dimension ref="B2:B10"/>
   <sheetViews>

</xml_diff>

<commit_message>
FreeCodeCamp article about SQLi added.
</commit_message>
<xml_diff>
--- a/Hacking Resources.xlsx
+++ b/Hacking Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FD2F7B-88AC-4F6C-901D-E8946B96BCC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7170D5D1-0804-48F9-8599-7905ADEDD303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
   </bookViews>
   <sheets>
     <sheet name="Github" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,9 @@
     <sheet name="Udacity" sheetId="5" r:id="rId4"/>
     <sheet name="Pentester Lab" sheetId="6" r:id="rId5"/>
     <sheet name="Youtube" sheetId="7" r:id="rId6"/>
-    <sheet name="Udemy" sheetId="2" r:id="rId7"/>
+    <sheet name="Tools" sheetId="8" r:id="rId7"/>
+    <sheet name="Udemy" sheetId="2" r:id="rId8"/>
+    <sheet name="Article" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>5 Useful GitHub Repositories #Shorts</t>
   </si>
@@ -169,6 +171,24 @@
   </si>
   <si>
     <t>OWASP Top 10 2017</t>
+  </si>
+  <si>
+    <t>https://github.com/dnoiz1/git-money</t>
+  </si>
+  <si>
+    <t>https://github.com/evilpacket/DVCS-Pillage</t>
+  </si>
+  <si>
+    <t>https://github.com/internetwache/GitTools</t>
+  </si>
+  <si>
+    <t>GIT leak Tools</t>
+  </si>
+  <si>
+    <t>https://www.freecodecamp.org/news/what-is-sql-injection-how-to-prevent-it/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FreeCodeCamp - SQL Injection </t>
   </si>
 </sst>
 </file>
@@ -830,7 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771B96C1-7ABF-46C5-9549-9CBFA9D2AE30}">
   <dimension ref="B2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -854,6 +874,49 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5DBA8C-2D26-45EF-8E01-0CE19B55241A}">
+  <dimension ref="B2:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="71.109375" customWidth="1"/>
+    <col min="3" max="3" width="62.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7831D5FA-64AA-4534-9A47-34375D983CF8}">
   <dimension ref="B2:B10"/>
   <sheetViews>
@@ -895,4 +958,31 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49270960-A31D-4C4E-A040-944256B8F4F1}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="71" customWidth="1"/>
+    <col min="3" max="3" width="97.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Networking for Web Developers by Udacity course added.
</commit_message>
<xml_diff>
--- a/Hacking Resources.xlsx
+++ b/Hacking Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7170D5D1-0804-48F9-8599-7905ADEDD303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C3813D-2030-455A-96C2-5F09CADC879D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
   </bookViews>
   <sheets>
     <sheet name="Github" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>5 Useful GitHub Repositories #Shorts</t>
   </si>
@@ -189,13 +189,19 @@
   </si>
   <si>
     <t xml:space="preserve">FreeCodeCamp - SQL Injection </t>
+  </si>
+  <si>
+    <t>https://www.udacity.com/course/networking-for-web-developers--ud256</t>
+  </si>
+  <si>
+    <t>Networking for Web Developers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +230,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2E3D49"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -246,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -255,6 +267,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -705,10 +720,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C93B1D4-544A-4029-B432-105DE78F91FA}">
-  <dimension ref="B2:C18"/>
+  <dimension ref="B2:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,8 +804,17 @@
         <v>35</v>
       </c>
     </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -964,7 +988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49270960-A31D-4C4E-A040-944256B8F4F1}">
   <dimension ref="B2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
HackTheBox Academy Link Added.
</commit_message>
<xml_diff>
--- a/Hacking Resources.xlsx
+++ b/Hacking Resources.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C3813D-2030-455A-96C2-5F09CADC879D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C291D19-94EC-43A0-94D3-D211977FD73F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{B48250E6-EC0C-409A-A259-AD73D3595A60}"/>
   </bookViews>
   <sheets>
     <sheet name="Github" sheetId="1" r:id="rId1"/>
     <sheet name="Hacker One" sheetId="3" r:id="rId2"/>
     <sheet name="Android" sheetId="4" r:id="rId3"/>
     <sheet name="Udacity" sheetId="5" r:id="rId4"/>
-    <sheet name="Pentester Lab" sheetId="6" r:id="rId5"/>
-    <sheet name="Youtube" sheetId="7" r:id="rId6"/>
-    <sheet name="Tools" sheetId="8" r:id="rId7"/>
-    <sheet name="Udemy" sheetId="2" r:id="rId8"/>
-    <sheet name="Article" sheetId="9" r:id="rId9"/>
+    <sheet name="CTF" sheetId="10" r:id="rId5"/>
+    <sheet name="HackTheBox" sheetId="11" r:id="rId6"/>
+    <sheet name="Pentester Lab" sheetId="6" r:id="rId7"/>
+    <sheet name="Youtube" sheetId="7" r:id="rId8"/>
+    <sheet name="Tools" sheetId="8" r:id="rId9"/>
+    <sheet name="Udemy" sheetId="2" r:id="rId10"/>
+    <sheet name="Article" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>5 Useful GitHub Repositories #Shorts</t>
   </si>
@@ -195,6 +197,18 @@
   </si>
   <si>
     <t>Networking for Web Developers</t>
+  </si>
+  <si>
+    <t>https://ctftime.org/event/list/upcoming</t>
+  </si>
+  <si>
+    <t>ALL CTF DETAILS</t>
+  </si>
+  <si>
+    <t>https://academy.hackthebox.eu/dashboard</t>
+  </si>
+  <si>
+    <t>Academy</t>
   </si>
 </sst>
 </file>
@@ -647,6 +661,77 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7831D5FA-64AA-4534-9A47-34375D983CF8}">
+  <dimension ref="B2:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="133.33203125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49270960-A31D-4C4E-A040-944256B8F4F1}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="71" customWidth="1"/>
+    <col min="3" max="3" width="97.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A7D2AF-9BAA-4A2D-A98D-3D7CE70D9BEB}">
   <dimension ref="B2:C4"/>
@@ -722,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C93B1D4-544A-4029-B432-105DE78F91FA}">
   <dimension ref="B2:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -819,6 +904,60 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725F99CC-2681-4DA7-B94D-E76A241AA5E8}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="53.21875" customWidth="1"/>
+    <col min="3" max="3" width="97.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282C834A-71E8-4015-AE77-141794C20CDB}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="53.33203125" customWidth="1"/>
+    <col min="3" max="3" width="97.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114BAD3-2286-4A06-9E26-58D1E6259D0C}">
   <dimension ref="B2:C8"/>
   <sheetViews>
@@ -870,7 +1009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771B96C1-7ABF-46C5-9549-9CBFA9D2AE30}">
   <dimension ref="B2:C2"/>
   <sheetViews>
@@ -897,7 +1036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5DBA8C-2D26-45EF-8E01-0CE19B55241A}">
   <dimension ref="B2:C6"/>
   <sheetViews>
@@ -938,75 +1077,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7831D5FA-64AA-4534-9A47-34375D983CF8}">
-  <dimension ref="B2:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="133.33203125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49270960-A31D-4C4E-A040-944256B8F4F1}">
-  <dimension ref="B2:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="71" customWidth="1"/>
-    <col min="3" max="3" width="97.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>